<commit_message>
added MCA data wrangling
</commit_message>
<xml_diff>
--- a/intermediary/northstar/percent_changes_districts_19_22_25.xlsx
+++ b/intermediary/northstar/percent_changes_districts_19_22_25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssachen/Desktop/Projects/mn-reformer/test-scores-2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssachen/Desktop/Projects/mn-reformer/test-scores-2025/intermediary/northstar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D3276-1CFF-B04F-9AFD-2B16809029BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9019DA-6A11-1C44-9698-0C7817D199D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="16720" xr2:uid="{E4A3B912-1F0E-BC49-B1C5-0F5278B60E04}"/>
+    <workbookView xWindow="-18100" yWindow="-3100" windowWidth="21140" windowHeight="17160" xr2:uid="{E4A3B912-1F0E-BC49-B1C5-0F5278B60E04}"/>
   </bookViews>
   <sheets>
     <sheet name="percent_changes_districts_19_22" sheetId="1" r:id="rId1"/>
@@ -2342,7 +2342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2457,6 +2457,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2502,7 +2511,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2513,6 +2522,12 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2894,7 +2909,7 @@
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="131" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="K50" sqref="K50"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2933,122 +2948,122 @@
     <col min="38" max="38" width="7.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="13" t="s">
         <v>29</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="13" t="s">
         <v>33</v>
       </c>
       <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="13" t="s">
         <v>37</v>
       </c>
       <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="S1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="V1" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="10" t="s">
         <v>25</v>
       </c>
       <c r="AL1" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="10" t="s">
         <v>646</v>
       </c>
     </row>
@@ -5838,122 +5853,122 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>821</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>320</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>320</v>
+        <v>38</v>
       </c>
       <c r="E26" s="6">
-        <v>1039</v>
+        <v>1186</v>
       </c>
       <c r="F26" s="4">
-        <v>0.95379999999999998</v>
+        <v>0.92920000000000003</v>
       </c>
       <c r="G26" s="5">
-        <v>0.46970000000000001</v>
+        <v>0.44519999999999998</v>
       </c>
       <c r="H26" t="s">
-        <v>320</v>
+        <v>38</v>
       </c>
       <c r="I26" s="6">
+        <v>1054</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.91839999999999999</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0.29980000000000001</v>
+      </c>
+      <c r="L26" t="s">
+        <v>38</v>
+      </c>
+      <c r="M26" s="6">
         <v>989</v>
       </c>
-      <c r="J26" s="4">
-        <v>0.94240000000000002</v>
-      </c>
-      <c r="K26" s="5">
-        <v>0.43480000000000002</v>
-      </c>
-      <c r="L26" t="s">
-        <v>320</v>
-      </c>
-      <c r="M26" s="6">
-        <v>987</v>
-      </c>
       <c r="N26" s="4">
-        <v>0.94430000000000003</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="O26" s="5">
-        <v>0.51270000000000004</v>
+        <v>0.44290000000000002</v>
       </c>
       <c r="P26" t="s">
-        <v>320</v>
+        <v>38</v>
       </c>
       <c r="Q26" s="2">
-        <v>19.71</v>
+        <v>56.62</v>
       </c>
       <c r="R26" s="8">
-        <v>21.42</v>
+        <v>56.96</v>
       </c>
       <c r="S26">
-        <v>90.51</v>
+        <v>96.92</v>
       </c>
       <c r="T26" s="2">
-        <v>19.29</v>
+        <v>53.62</v>
       </c>
       <c r="U26" s="8">
-        <v>22.92</v>
+        <v>50</v>
       </c>
       <c r="V26">
-        <v>87.9</v>
+        <v>96.15</v>
       </c>
       <c r="W26" s="2">
-        <v>21.7</v>
+        <v>58.59</v>
       </c>
       <c r="X26" s="8">
-        <v>26.99</v>
+        <v>54.05</v>
       </c>
       <c r="Y26" t="s">
         <v>39</v>
       </c>
       <c r="Z26">
-        <v>-2.1308980213089902E-2</v>
+        <v>-5.2984811020840697E-2</v>
       </c>
       <c r="AA26">
-        <v>-0.42000000000000198</v>
+        <v>-3</v>
       </c>
       <c r="AB26">
-        <v>0.124935199585277</v>
+        <v>9.2689295039164593E-2</v>
       </c>
       <c r="AC26">
-        <v>2.41</v>
+        <v>4.9700000000000104</v>
       </c>
       <c r="AD26">
-        <v>0.10096397767630599</v>
+        <v>3.4793359237018803E-2</v>
       </c>
       <c r="AE26">
-        <v>1.99</v>
+        <v>1.97000000000001</v>
       </c>
       <c r="AF26">
-        <v>7.0028011204481794E-2</v>
+        <v>-0.12219101123595499</v>
       </c>
       <c r="AG26">
-        <v>1.5</v>
+        <v>-6.96</v>
       </c>
       <c r="AH26">
-        <v>0.17757417102966799</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="AI26">
-        <v>4.07</v>
+        <v>4.05</v>
       </c>
       <c r="AJ26">
-        <v>0.26003734827264202</v>
+        <v>-5.1088483146067502E-2</v>
       </c>
       <c r="AK26">
-        <v>5.57</v>
+        <v>-2.91</v>
       </c>
       <c r="AL26" t="s">
-        <v>320</v>
+        <v>38</v>
       </c>
       <c r="AN26">
         <f>MAX(AK26,AE26)</f>
-        <v>5.57</v>
+        <v>1.97000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
@@ -6074,122 +6089,122 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2397</v>
+        <v>287</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>405</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
-        <v>405</v>
+        <v>153</v>
       </c>
       <c r="E28" s="6">
-        <v>1026</v>
+        <v>1075</v>
       </c>
       <c r="F28" s="4">
-        <v>0.75629999999999997</v>
+        <v>0.4335</v>
       </c>
       <c r="G28" s="5">
-        <v>0.32940000000000003</v>
+        <v>0.56189999999999996</v>
       </c>
       <c r="H28" t="s">
-        <v>405</v>
+        <v>153</v>
       </c>
       <c r="I28" s="6">
-        <v>946</v>
+        <v>800</v>
       </c>
       <c r="J28" s="4">
-        <v>0.75790000000000002</v>
+        <v>0.39379999999999998</v>
       </c>
       <c r="K28" s="5">
-        <v>0.26529999999999998</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="L28" t="s">
-        <v>405</v>
+        <v>153</v>
       </c>
       <c r="M28" s="6">
-        <v>908</v>
+        <v>927</v>
       </c>
       <c r="N28" s="4">
-        <v>0.75</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="O28" s="5">
-        <v>0.37669999999999998</v>
+        <v>0.60409999999999997</v>
       </c>
       <c r="P28" t="s">
-        <v>405</v>
+        <v>153</v>
       </c>
       <c r="Q28" s="2">
-        <v>52.86</v>
+        <v>3.93</v>
       </c>
       <c r="R28" s="8">
-        <v>52.15</v>
+        <v>7.69</v>
       </c>
       <c r="S28">
-        <v>92.84</v>
+        <v>48.86</v>
       </c>
       <c r="T28" s="2">
-        <v>51.02</v>
+        <v>2.34</v>
       </c>
       <c r="U28" s="8">
-        <v>49.89</v>
+        <v>5.82</v>
       </c>
       <c r="V28">
-        <v>82.49</v>
+        <v>25.32</v>
       </c>
       <c r="W28" s="2">
-        <v>57.07</v>
+        <v>3.94</v>
       </c>
       <c r="X28" s="8">
-        <v>57.33</v>
+        <v>5.04</v>
       </c>
       <c r="Y28" t="s">
         <v>39</v>
       </c>
       <c r="Z28">
-        <v>-3.4808929247067702E-2</v>
+        <v>-0.40458015267175601</v>
       </c>
       <c r="AA28">
-        <v>-1.84</v>
+        <v>-1.59</v>
       </c>
       <c r="AB28">
-        <v>0.118580948647589</v>
+        <v>0.683760683760684</v>
       </c>
       <c r="AC28">
-        <v>6.05</v>
+        <v>1.6</v>
       </c>
       <c r="AD28">
-        <v>7.9644343548997396E-2</v>
+        <v>2.54452926208646E-3</v>
       </c>
       <c r="AE28">
-        <v>4.21</v>
+        <v>9.9999999999997903E-3</v>
       </c>
       <c r="AF28">
-        <v>-4.3336529242569498E-2</v>
+        <v>-0.24317295188556601</v>
       </c>
       <c r="AG28">
-        <v>-2.2599999999999998</v>
+        <v>-1.87</v>
       </c>
       <c r="AH28">
-        <v>0.14912808177991599</v>
+        <v>-0.134020618556701</v>
       </c>
       <c r="AI28">
-        <v>7.44</v>
+        <v>-0.78</v>
       </c>
       <c r="AJ28">
-        <v>9.9328859060402702E-2</v>
+        <v>-0.34460338101430399</v>
       </c>
       <c r="AK28">
-        <v>5.18</v>
+        <v>-2.65</v>
       </c>
       <c r="AL28" t="s">
-        <v>405</v>
+        <v>153</v>
       </c>
       <c r="AN28">
         <f>MAX(AK28,AE28)</f>
-        <v>5.18</v>
+        <v>9.9999999999997903E-3</v>
       </c>
     </row>
     <row r="29" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
@@ -7470,122 +7485,122 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>484</v>
+        <v>2397</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>210</v>
+        <v>405</v>
       </c>
       <c r="D40" t="s">
-        <v>210</v>
+        <v>405</v>
       </c>
       <c r="E40" s="6">
-        <v>1195</v>
+        <v>1026</v>
       </c>
       <c r="F40" s="4">
-        <v>0.96819999999999995</v>
+        <v>0.75629999999999997</v>
       </c>
       <c r="G40" s="5">
-        <v>0.34310000000000002</v>
+        <v>0.32940000000000003</v>
       </c>
       <c r="H40" t="s">
-        <v>210</v>
+        <v>405</v>
       </c>
       <c r="I40" s="6">
-        <v>1249</v>
+        <v>946</v>
       </c>
       <c r="J40" s="4">
-        <v>0.95440000000000003</v>
+        <v>0.75790000000000002</v>
       </c>
       <c r="K40" s="5">
-        <v>0.2482</v>
+        <v>0.26529999999999998</v>
       </c>
       <c r="L40" t="s">
-        <v>210</v>
+        <v>405</v>
       </c>
       <c r="M40" s="6">
-        <v>1214</v>
+        <v>908</v>
       </c>
       <c r="N40" s="4">
-        <v>0.95220000000000005</v>
+        <v>0.75</v>
       </c>
       <c r="O40" s="5">
-        <v>0.27510000000000001</v>
+        <v>0.37669999999999998</v>
       </c>
       <c r="P40" t="s">
-        <v>210</v>
+        <v>405</v>
       </c>
       <c r="Q40" s="2">
-        <v>63.63</v>
+        <v>52.86</v>
       </c>
       <c r="R40" s="8">
-        <v>60.56</v>
+        <v>52.15</v>
       </c>
       <c r="S40">
-        <v>89.81</v>
+        <v>92.84</v>
       </c>
       <c r="T40" s="2">
-        <v>54.34</v>
+        <v>51.02</v>
       </c>
       <c r="U40" s="8">
-        <v>50.75</v>
+        <v>49.89</v>
       </c>
       <c r="V40">
-        <v>77.58</v>
+        <v>82.49</v>
       </c>
       <c r="W40" s="2">
-        <v>63.98</v>
+        <v>57.07</v>
       </c>
       <c r="X40" s="8">
-        <v>63.07</v>
+        <v>57.33</v>
       </c>
       <c r="Y40" t="s">
         <v>39</v>
       </c>
       <c r="Z40">
-        <v>-0.146000314317146</v>
+        <v>-3.4808929247067702E-2</v>
       </c>
       <c r="AA40">
-        <v>-9.2899999999999991</v>
+        <v>-1.84</v>
       </c>
       <c r="AB40">
-        <v>0.17740154582259801</v>
+        <v>0.118580948647589</v>
       </c>
       <c r="AC40">
-        <v>9.6399999999999899</v>
+        <v>6.05</v>
       </c>
       <c r="AD40">
-        <v>5.5005500550054098E-3</v>
+        <v>7.9644343548997396E-2</v>
       </c>
       <c r="AE40">
-        <v>0.34999999999999398</v>
+        <v>4.21</v>
       </c>
       <c r="AF40">
-        <v>-0.16198811096433299</v>
+        <v>-4.3336529242569498E-2</v>
       </c>
       <c r="AG40">
-        <v>-9.81</v>
+        <v>-2.2599999999999998</v>
       </c>
       <c r="AH40">
-        <v>0.24275862068965501</v>
+        <v>0.14912808177991599</v>
       </c>
       <c r="AI40">
-        <v>12.32</v>
+        <v>7.44</v>
       </c>
       <c r="AJ40">
-        <v>4.1446499339497997E-2</v>
+        <v>9.9328859060402702E-2</v>
       </c>
       <c r="AK40">
-        <v>2.5099999999999998</v>
+        <v>5.18</v>
       </c>
       <c r="AL40" t="s">
-        <v>211</v>
+        <v>405</v>
       </c>
       <c r="AN40">
         <f>MAX(AK40,AE40)</f>
-        <v>2.5099999999999998</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="41" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
@@ -7706,122 +7721,122 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1</v>
+        <v>821</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="E42" s="6">
-        <v>1186</v>
+        <v>1039</v>
       </c>
       <c r="F42" s="4">
-        <v>0.92920000000000003</v>
+        <v>0.95379999999999998</v>
       </c>
       <c r="G42" s="5">
-        <v>0.44519999999999998</v>
+        <v>0.46970000000000001</v>
       </c>
       <c r="H42" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="I42" s="6">
-        <v>1054</v>
+        <v>989</v>
       </c>
       <c r="J42" s="4">
-        <v>0.91839999999999999</v>
+        <v>0.94240000000000002</v>
       </c>
       <c r="K42" s="5">
-        <v>0.29980000000000001</v>
+        <v>0.43480000000000002</v>
       </c>
       <c r="L42" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="M42" s="6">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="N42" s="4">
-        <v>0.91300000000000003</v>
+        <v>0.94430000000000003</v>
       </c>
       <c r="O42" s="5">
-        <v>0.44290000000000002</v>
+        <v>0.51270000000000004</v>
       </c>
       <c r="P42" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="Q42" s="2">
-        <v>56.62</v>
+        <v>19.71</v>
       </c>
       <c r="R42" s="8">
-        <v>56.96</v>
+        <v>21.42</v>
       </c>
       <c r="S42">
-        <v>96.92</v>
+        <v>90.51</v>
       </c>
       <c r="T42" s="2">
-        <v>53.62</v>
+        <v>19.29</v>
       </c>
       <c r="U42" s="8">
-        <v>50</v>
+        <v>22.92</v>
       </c>
       <c r="V42">
-        <v>96.15</v>
+        <v>87.9</v>
       </c>
       <c r="W42" s="2">
-        <v>58.59</v>
+        <v>21.7</v>
       </c>
       <c r="X42" s="8">
-        <v>54.05</v>
+        <v>26.99</v>
       </c>
       <c r="Y42" t="s">
         <v>39</v>
       </c>
       <c r="Z42">
-        <v>-5.2984811020840697E-2</v>
+        <v>-2.1308980213089902E-2</v>
       </c>
       <c r="AA42">
-        <v>-3</v>
+        <v>-0.42000000000000198</v>
       </c>
       <c r="AB42">
-        <v>9.2689295039164593E-2</v>
+        <v>0.124935199585277</v>
       </c>
       <c r="AC42">
-        <v>4.9700000000000104</v>
+        <v>2.41</v>
       </c>
       <c r="AD42">
-        <v>3.4793359237018803E-2</v>
+        <v>0.10096397767630599</v>
       </c>
       <c r="AE42">
-        <v>1.97000000000001</v>
+        <v>1.99</v>
       </c>
       <c r="AF42">
-        <v>-0.12219101123595499</v>
+        <v>7.0028011204481794E-2</v>
       </c>
       <c r="AG42">
-        <v>-6.96</v>
+        <v>1.5</v>
       </c>
       <c r="AH42">
-        <v>8.1000000000000003E-2</v>
+        <v>0.17757417102966799</v>
       </c>
       <c r="AI42">
-        <v>4.05</v>
+        <v>4.07</v>
       </c>
       <c r="AJ42">
-        <v>-5.1088483146067502E-2</v>
+        <v>0.26003734827264202</v>
       </c>
       <c r="AK42">
-        <v>-2.91</v>
+        <v>5.57</v>
       </c>
       <c r="AL42" t="s">
-        <v>38</v>
+        <v>320</v>
       </c>
       <c r="AN42">
         <f>MAX(AK42,AE42)</f>
-        <v>1.97000000000001</v>
+        <v>5.57</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.2">
@@ -8526,242 +8541,242 @@
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>116</v>
+        <v>484</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="E49" s="6">
-        <v>1164</v>
+        <v>1195</v>
       </c>
       <c r="F49" s="4">
-        <v>0.94930000000000003</v>
+        <v>0.96819999999999995</v>
       </c>
       <c r="G49" s="5">
-        <v>0.4244</v>
+        <v>0.34310000000000002</v>
       </c>
       <c r="H49" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="I49" s="6">
-        <v>1228</v>
+        <v>1249</v>
       </c>
       <c r="J49" s="4">
-        <v>0.94379999999999997</v>
+        <v>0.95440000000000003</v>
       </c>
       <c r="K49" s="5">
-        <v>0.39410000000000001</v>
+        <v>0.2482</v>
       </c>
       <c r="L49" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="M49" s="6">
-        <v>1324</v>
+        <v>1214</v>
       </c>
       <c r="N49" s="4">
-        <v>0.92300000000000004</v>
+        <v>0.95220000000000005</v>
       </c>
       <c r="O49" s="5">
-        <v>0.37390000000000001</v>
+        <v>0.27510000000000001</v>
       </c>
       <c r="P49" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="Q49" s="2">
-        <v>45.51</v>
+        <v>63.63</v>
       </c>
       <c r="R49" s="8">
-        <v>59.29</v>
+        <v>60.56</v>
       </c>
       <c r="S49">
-        <v>78.52</v>
+        <v>89.81</v>
       </c>
       <c r="T49" s="2">
-        <v>45.69</v>
+        <v>54.34</v>
       </c>
       <c r="U49" s="8">
-        <v>51.93</v>
+        <v>50.75</v>
       </c>
       <c r="V49">
-        <v>64.16</v>
+        <v>77.58</v>
       </c>
       <c r="W49" s="2">
-        <v>47.25</v>
+        <v>63.98</v>
       </c>
       <c r="X49" s="8">
-        <v>48.95</v>
+        <v>63.07</v>
       </c>
       <c r="Y49" t="s">
         <v>39</v>
       </c>
       <c r="Z49">
-        <v>3.9551746868819997E-3</v>
+        <v>-0.146000314317146</v>
       </c>
       <c r="AA49">
-        <v>0.18</v>
+        <v>-9.2899999999999991</v>
       </c>
       <c r="AB49">
-        <v>3.4143138542350703E-2</v>
+        <v>0.17740154582259801</v>
       </c>
       <c r="AC49">
-        <v>1.56</v>
+        <v>9.6399999999999899</v>
       </c>
       <c r="AD49">
-        <v>3.82333553065261E-2</v>
+        <v>5.5005500550054098E-3</v>
       </c>
       <c r="AE49">
-        <v>1.74</v>
+        <v>0.34999999999999398</v>
       </c>
       <c r="AF49">
-        <v>-0.124135604655085</v>
+        <v>-0.16198811096433299</v>
       </c>
       <c r="AG49">
-        <v>-7.36</v>
+        <v>-9.81</v>
       </c>
       <c r="AH49">
-        <v>-5.7384941267090303E-2</v>
+        <v>0.24275862068965501</v>
       </c>
       <c r="AI49">
-        <v>-2.98</v>
+        <v>12.32</v>
       </c>
       <c r="AJ49">
-        <v>-0.174397031539889</v>
+        <v>4.1446499339497997E-2</v>
       </c>
       <c r="AK49">
-        <v>-10.34</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="AL49" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="AN49">
         <f>MAX(AK49,AE49)</f>
-        <v>1.74</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>287</v>
+        <v>116</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="E50" s="6">
-        <v>1075</v>
+        <v>1164</v>
       </c>
       <c r="F50" s="4">
-        <v>0.4335</v>
+        <v>0.94930000000000003</v>
       </c>
       <c r="G50" s="5">
-        <v>0.56189999999999996</v>
+        <v>0.4244</v>
       </c>
       <c r="H50" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="I50" s="6">
-        <v>800</v>
+        <v>1228</v>
       </c>
       <c r="J50" s="4">
-        <v>0.39379999999999998</v>
+        <v>0.94379999999999997</v>
       </c>
       <c r="K50" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.39410000000000001</v>
       </c>
       <c r="L50" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="M50" s="6">
-        <v>927</v>
+        <v>1324</v>
       </c>
       <c r="N50" s="4">
-        <v>0.33329999999999999</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="O50" s="5">
-        <v>0.60409999999999997</v>
+        <v>0.37390000000000001</v>
       </c>
       <c r="P50" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="Q50" s="2">
-        <v>3.93</v>
+        <v>45.51</v>
       </c>
       <c r="R50" s="8">
-        <v>7.69</v>
+        <v>59.29</v>
       </c>
       <c r="S50">
-        <v>48.86</v>
+        <v>78.52</v>
       </c>
       <c r="T50" s="2">
-        <v>2.34</v>
+        <v>45.69</v>
       </c>
       <c r="U50" s="8">
-        <v>5.82</v>
+        <v>51.93</v>
       </c>
       <c r="V50">
-        <v>25.32</v>
+        <v>64.16</v>
       </c>
       <c r="W50" s="2">
-        <v>3.94</v>
+        <v>47.25</v>
       </c>
       <c r="X50" s="8">
-        <v>5.04</v>
+        <v>48.95</v>
       </c>
       <c r="Y50" t="s">
         <v>39</v>
       </c>
       <c r="Z50">
-        <v>-0.40458015267175601</v>
+        <v>3.9551746868819997E-3</v>
       </c>
       <c r="AA50">
-        <v>-1.59</v>
+        <v>0.18</v>
       </c>
       <c r="AB50">
-        <v>0.683760683760684</v>
+        <v>3.4143138542350703E-2</v>
       </c>
       <c r="AC50">
-        <v>1.6</v>
+        <v>1.56</v>
       </c>
       <c r="AD50">
-        <v>2.54452926208646E-3</v>
+        <v>3.82333553065261E-2</v>
       </c>
       <c r="AE50">
-        <v>9.9999999999997903E-3</v>
+        <v>1.74</v>
       </c>
       <c r="AF50">
-        <v>-0.24317295188556601</v>
+        <v>-0.124135604655085</v>
       </c>
       <c r="AG50">
-        <v>-1.87</v>
+        <v>-7.36</v>
       </c>
       <c r="AH50">
-        <v>-0.134020618556701</v>
+        <v>-5.7384941267090303E-2</v>
       </c>
       <c r="AI50">
-        <v>-0.78</v>
+        <v>-2.98</v>
       </c>
       <c r="AJ50">
-        <v>-0.34460338101430399</v>
+        <v>-0.174397031539889</v>
       </c>
       <c r="AK50">
-        <v>-2.65</v>
+        <v>-10.34</v>
       </c>
       <c r="AL50" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="AN50">
         <f>MAX(AK50,AE50)</f>
-        <v>9.9999999999997903E-3</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="51" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
@@ -57033,8 +57048,8 @@
         <customFilter operator="greaterThan" val="0"/>
       </customFilters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A26:AN456">
-      <sortCondition descending="1" ref="AN1:AN462"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A26:AN50">
+      <sortCondition ref="C1:C462"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AN1">
@@ -57046,7 +57061,7 @@
       <selection pane="topRight" activeCell="AN40" sqref="AN40"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-      <autoFilter ref="A1:AN462" xr:uid="{1E4691F1-7618-5B4D-B4F2-5FB05C5EC2D5}">
+      <autoFilter ref="A1:AN462" xr:uid="{E2C18B70-ADEA-A044-9BA8-79839C999DCC}">
         <filterColumn colId="2">
           <customFilters>
             <customFilter val="*district*"/>

</xml_diff>